<commit_message>
make all money columns a relative counterpart
</commit_message>
<xml_diff>
--- a/Scripts/DataScience/PenztargepAdatok/grand-penztargep-datummal.xlsx
+++ b/Scripts/DataScience/PenztargepAdatok/grand-penztargep-datummal.xlsx
@@ -406,12 +406,16 @@
   <dimension ref="A1:I817"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -24109,5 +24113,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>